<commit_message>
Added possibility to adding flmc to table with the same name through the special interface
</commit_message>
<xml_diff>
--- a/bases/lfmc.xlsx
+++ b/bases/lfmc.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,10 +476,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>defaultA1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -518,10 +516,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>defaultB1</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -560,10 +556,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>defaultC1</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -602,10 +596,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>defaultD1</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -644,10 +636,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>defaultE1</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -686,10 +676,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>default</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -728,10 +716,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>default</t>
-        </is>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -770,10 +756,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>default</t>
-        </is>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -812,10 +796,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>default</t>
-        </is>
+      <c r="A10" t="n">
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -854,10 +836,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>default</t>
-        </is>
+      <c r="A11" t="n">
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -896,10 +876,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>default</t>
-        </is>
+      <c r="A12" t="n">
+        <v>11</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -938,10 +916,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>default</t>
-        </is>
+      <c r="A13" t="n">
+        <v>12</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -980,10 +956,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>default</t>
-        </is>
+      <c r="A14" t="n">
+        <v>13</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1022,10 +996,8 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>default</t>
-        </is>
+      <c r="A15" t="n">
+        <v>14</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1064,10 +1036,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>default</t>
-        </is>
+      <c r="A16" t="n">
+        <v>15</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1106,10 +1076,8 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>default</t>
-        </is>
+      <c r="A17" t="n">
+        <v>16</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1148,10 +1116,8 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>default</t>
-        </is>
+      <c r="A18" t="n">
+        <v>17</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1190,10 +1156,8 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>default</t>
-        </is>
+      <c r="A19" t="n">
+        <v>18</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1228,6 +1192,566 @@
       <c r="H19" t="inlineStr">
         <is>
           <t>default</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>hsdfew</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>hsdfew</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>fdh3e</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>fdh3e</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>dfh24</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>fdh3e</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>fdh3e</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>fdh3e</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>fdh3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>bfd</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>bfd</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>gfncvnfd</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>bfd</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>bfd</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>bfd</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>bfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>hdfw</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>hdfw</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>rher</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>hdfw</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>hdfw</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>hdfw</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>hdfw</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>hdfw</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>hdfw</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>rher</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>hdfw</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>hdfw</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>hdfw</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>hdfw</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>fsdg</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>fsdg</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>sgsg</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>fsdg</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>fsdg</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>fsdg</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>fsdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>wert</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>wert</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>hdf</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>wert</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>wert</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>wert</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>wert</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>gsdf</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>gfdhjy</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>sdfcvsdg</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>fdgsdg</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>bcvbsdf</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>asfvcx</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>sfcxv</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>sdfhtkuy</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>nvbndfghvbn</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>fgdcv</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>fgdfbcvb</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>fdgfdvc</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>bfgdfg</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>bdsdgg</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>sdfhtkuy</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>nvbndfghvbn</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>fgdcv</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>fgdfbcvb</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>fdgfdvc</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>bfgdfg</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>bdsdgg</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>sdgcxv</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>sdfxc</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>vasfsd</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>xcvsadf</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>vxcasf</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>bvfgdfj</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>cvsdfs</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added possibility to view flmc params in the form before changing
</commit_message>
<xml_diff>
--- a/bases/lfmc.xlsx
+++ b/bases/lfmc.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1755,6 +1755,46 @@
         </is>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>fsadfs</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>gcxvsdf</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>cbxsdf</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>xccbc</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>asdsdgc</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>vasafsd</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>xcvdss</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added possibility to change flmc params, fixed some bugs and added information about screen scale into window named helpUI
</commit_message>
<xml_diff>
--- a/bases/lfmc.xlsx
+++ b/bases/lfmc.xlsx
@@ -481,7 +481,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>defaultA2</t>
+          <t>asfgqw</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -516,8 +516,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -526,12 +528,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>defaultB3</t>
+          <t>asfagsad</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>defaultB4</t>
+          <t>hsdfqvxz</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -591,7 +593,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>defaultC8</t>
+          <t>fdsgcxvwsg</t>
         </is>
       </c>
     </row>
@@ -616,7 +618,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>defaultD5</t>
+          <t>sfsdfsdff</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -631,7 +633,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>defaultD8</t>
+          <t>defaultD8fd</t>
         </is>
       </c>
     </row>
@@ -651,7 +653,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>defaultE4</t>
+          <t>фыыфвфы</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">

</xml_diff>